<commit_message>
Fixed excel creation. Wrong data removed
</commit_message>
<xml_diff>
--- a/Data Sources/Excel/Teams-Info.xlsx
+++ b/Data Sources/Excel/Teams-Info.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Team</t>
   </si>
@@ -50,13 +50,13 @@
     <t>Total Costs</t>
   </si>
   <si>
-    <t>Cska Sofia</t>
-  </si>
-  <si>
-    <t>Stoicho Stoev</t>
-  </si>
-  <si>
-    <t>Michael Chorni</t>
+    <t>CSKA</t>
+  </si>
+  <si>
+    <t>Petar Ivanov</t>
+  </si>
+  <si>
+    <t>Minko Goshev</t>
   </si>
   <si>
     <t>Red</t>
@@ -74,7 +74,7 @@
     <t>20680</t>
   </si>
   <si>
-    <t>Levski Sofia</t>
+    <t>Levski</t>
   </si>
   <si>
     <t>Ivan Ivanov</t>
@@ -86,13 +86,82 @@
     <t>Blue</t>
   </si>
   <si>
-    <t>0</t>
+    <t>6</t>
   </si>
   <si>
     <t>350</t>
   </si>
   <si>
     <t>150</t>
+  </si>
+  <si>
+    <t>3000</t>
+  </si>
+  <si>
+    <t>Beroe</t>
+  </si>
+  <si>
+    <t>Petar Hubchev</t>
+  </si>
+  <si>
+    <t>Maritza Iztok 2 Pesho</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>9600</t>
+  </si>
+  <si>
+    <t>Ludogorets</t>
+  </si>
+  <si>
+    <t>Petar Angelov</t>
+  </si>
+  <si>
+    <t>Petio Andreev</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>180</t>
+  </si>
+  <si>
+    <t>12480</t>
+  </si>
+  <si>
+    <t>Litex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valio </t>
+  </si>
+  <si>
+    <t>Programista Gosho</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>250</t>
+  </si>
+  <si>
+    <t>130</t>
+  </si>
+  <si>
+    <t>9880</t>
   </si>
 </sst>
 </file>
@@ -158,15 +227,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0" view="pageLayout"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.4939836774554" customWidth="1"/>
-    <col min="2" max="2" width="13.3334546770368" customWidth="1"/>
-    <col min="3" max="3" width="14.693108694894" customWidth="1"/>
+    <col min="1" max="1" width="11.2719781058175" customWidth="1"/>
+    <col min="2" max="2" width="14.3053676060268" customWidth="1"/>
+    <col min="3" max="3" width="20.2473297119141" customWidth="1"/>
     <col min="4" max="4" width="12.1988754272461" customWidth="1"/>
     <col min="5" max="5" width="12.3758653913225" customWidth="1"/>
     <col min="6" max="6" width="13.0562046595982" customWidth="1"/>
@@ -233,10 +302,10 @@
         <v>15</v>
       </c>
       <c r="F2" s="3">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G2" s="3">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>16</v>
@@ -271,10 +340,10 @@
         <v>23</v>
       </c>
       <c r="F3" s="3">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3" s="3">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>24</v>
@@ -289,7 +358,121 @@
         <v>26</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3">
+        <v>2</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="3">
+        <v>4</v>
+      </c>
+      <c r="G5" s="3">
+        <v>2</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="3">
+        <v>4</v>
+      </c>
+      <c r="G6" s="3">
+        <v>4</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
After teamwork defense commit. Minor fixes. Everything is working.
</commit_message>
<xml_diff>
--- a/Data Sources/Excel/Teams-Info.xlsx
+++ b/Data Sources/Excel/Teams-Info.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Team</t>
   </si>
@@ -62,40 +62,40 @@
     <t>Red</t>
   </si>
   <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>300</t>
+  </si>
+  <si>
+    <t>170</t>
+  </si>
+  <si>
+    <t>28200</t>
+  </si>
+  <si>
+    <t>Levski</t>
+  </si>
+  <si>
+    <t>Ivan Ivanov</t>
+  </si>
+  <si>
+    <t>Gosho Goshev</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
     <t>44</t>
   </si>
   <si>
-    <t>300</t>
-  </si>
-  <si>
-    <t>170</t>
-  </si>
-  <si>
-    <t>20680</t>
-  </si>
-  <si>
-    <t>Levski</t>
-  </si>
-  <si>
-    <t>Ivan Ivanov</t>
-  </si>
-  <si>
-    <t>Gosho Goshev</t>
-  </si>
-  <si>
-    <t>Blue</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
     <t>350</t>
   </si>
   <si>
     <t>150</t>
   </si>
   <si>
-    <t>3000</t>
+    <t>22000</t>
   </si>
   <si>
     <t>Beroe</t>
@@ -113,16 +113,13 @@
     <t>White</t>
   </si>
   <si>
-    <t>32</t>
-  </si>
-  <si>
     <t>200</t>
   </si>
   <si>
     <t>100</t>
   </si>
   <si>
-    <t>9600</t>
+    <t>18000</t>
   </si>
   <si>
     <t>Ludogorets</t>
@@ -134,13 +131,10 @@
     <t>Petio Andreev</t>
   </si>
   <si>
-    <t>26</t>
-  </si>
-  <si>
     <t>180</t>
   </si>
   <si>
-    <t>12480</t>
+    <t>21120</t>
   </si>
   <si>
     <t>Litex</t>
@@ -161,7 +155,7 @@
     <t>130</t>
   </si>
   <si>
-    <t>9880</t>
+    <t>16720</t>
   </si>
 </sst>
 </file>
@@ -384,30 +378,30 @@
         <v>2</v>
       </c>
       <c r="H4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>31</v>
@@ -422,33 +416,33 @@
         <v>2</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>32</v>
@@ -460,19 +454,19 @@
         <v>4</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="J6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>